<commit_message>
fixed issue drawign remote kinects on desktop
</commit_message>
<xml_diff>
--- a/03_Docs/ReactiveSpaces-Backlog.xlsx
+++ b/03_Docs/ReactiveSpaces-Backlog.xlsx
@@ -4599,7 +4599,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4755,14 +4755,14 @@
         <v>19</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G5" s="20">
         <v>41936</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="24" t="str">
         <f ca="1">IF(EXACT( E5, Pickers!$B$5), "done", _xlfn.DAYS(  G5, TODAY() ) )</f>
-        <v>-10</v>
+        <v>done</v>
       </c>
       <c r="I5" s="21">
         <f t="shared" si="0"/>
@@ -4788,14 +4788,14 @@
         <v>19</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G6" s="20">
         <v>41936</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="24" t="str">
         <f ca="1">IF(EXACT( E6, Pickers!$B$5), "done", _xlfn.DAYS(  G6, TODAY() ) )</f>
-        <v>-10</v>
+        <v>done</v>
       </c>
       <c r="I6" s="21">
         <f t="shared" si="0"/>
@@ -4821,14 +4821,14 @@
         <v>19</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G7" s="20">
         <v>41936</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="24" t="str">
         <f ca="1">IF(EXACT( E7, Pickers!$B$5), "done", _xlfn.DAYS(  G7, TODAY() ) )</f>
-        <v>-10</v>
+        <v>done</v>
       </c>
       <c r="I7" s="21">
         <f t="shared" si="0"/>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="H16" s="24">
         <f ca="1">IF(EXACT( E16, Pickers!$B$5), "done", _xlfn.DAYS(  G16, TODAY() ) )</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" si="0"/>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="H17" s="24">
         <f ca="1">IF(EXACT( E17, Pickers!$B$5), "done", _xlfn.DAYS(  G17, TODAY() ) )</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I17" s="21">
         <f t="shared" si="0"/>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="H19" s="24">
         <f ca="1">IF(EXACT( E19, Pickers!$B$5), "done", _xlfn.DAYS(  G19, TODAY() ) )</f>
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" si="0"/>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="H20" s="24">
         <f ca="1">IF(EXACT( E20, Pickers!$B$5), "done", _xlfn.DAYS(  G20, TODAY() ) )</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" si="0"/>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="H21" s="24">
         <f ca="1">IF(EXACT( E21, Pickers!$B$5), "done", _xlfn.DAYS(  G21, TODAY() ) )</f>
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="I21" s="21">
         <f t="shared" si="0"/>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="H22" s="24">
         <f ca="1">IF(EXACT( E22, Pickers!$B$5), "done", _xlfn.DAYS(  G22, TODAY() ) )</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="I22" s="21">
         <f t="shared" si="0"/>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="H23" s="24">
         <f ca="1">IF(EXACT( E23, Pickers!$B$5), "done", _xlfn.DAYS(  G23, TODAY() ) )</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I23" s="21">
         <f t="shared" si="0"/>
@@ -5390,7 +5390,7 @@
       </c>
       <c r="H24" s="24">
         <f ca="1">IF(EXACT( E24, Pickers!$B$5), "done", _xlfn.DAYS(  G24, TODAY() ) )</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I24" s="21">
         <f t="shared" si="0"/>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="H25" s="24">
         <f ca="1">IF(EXACT( E25, Pickers!$B$5), "done", _xlfn.DAYS(  G25, TODAY() ) )</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I25" s="21">
         <f t="shared" si="0"/>
@@ -5456,7 +5456,7 @@
       </c>
       <c r="H26" s="24">
         <f ca="1">IF(EXACT( E26, Pickers!$B$5), "done", _xlfn.DAYS(  G26, TODAY() ) )</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I26" s="21">
         <f t="shared" si="0"/>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="H27" s="24">
         <f ca="1">IF(EXACT( E27, Pickers!$B$5), "done", _xlfn.DAYS(  G27, TODAY() ) )</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I27" s="21">
         <f t="shared" si="0"/>
@@ -5522,7 +5522,7 @@
       </c>
       <c r="H28" s="24">
         <f ca="1">IF(EXACT( E28, Pickers!$B$5), "done", _xlfn.DAYS(  G28, TODAY() ) )</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I28" s="21">
         <f t="shared" si="0"/>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="H29" s="24">
         <f ca="1">IF(EXACT( E29, Pickers!$B$5), "done", _xlfn.DAYS(  G29, TODAY() ) )</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I29" s="21">
         <f t="shared" si="0"/>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="H30" s="24">
         <f ca="1">IF(EXACT( E30, Pickers!$B$5), "done", _xlfn.DAYS(  G30, TODAY() ) )</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="I30" s="21">
         <f t="shared" si="0"/>
@@ -5621,7 +5621,7 @@
       </c>
       <c r="H31" s="24">
         <f ca="1">IF(EXACT( E31, Pickers!$B$5), "done", _xlfn.DAYS(  G31, TODAY() ) )</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I31" s="21">
         <f t="shared" si="0"/>
@@ -5719,7 +5719,7 @@
       </c>
       <c r="H34" s="24">
         <f ca="1">IF(EXACT( E34, Pickers!$B$5), "done", _xlfn.DAYS(  G34, TODAY() ) )</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I34" s="21">
         <f t="shared" si="0"/>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="H35" s="24">
         <f ca="1">IF(EXACT( E35, Pickers!$B$5), "done", _xlfn.DAYS(  G35, TODAY() ) )</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I35" s="21">
         <f t="shared" si="0"/>
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H36" s="24">
         <f ca="1">IF(EXACT( E36, Pickers!$B$5), "done", _xlfn.DAYS(  G36, TODAY() ) )</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="I36" s="21">
         <f t="shared" si="0"/>
@@ -5818,7 +5818,7 @@
       </c>
       <c r="H37" s="24">
         <f ca="1">IF(EXACT( E37, Pickers!$B$5), "done", _xlfn.DAYS(  G37, TODAY() ) )</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I37" s="21">
         <f t="shared" si="0"/>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="H38" s="24">
         <f ca="1">IF(EXACT( E38, Pickers!$B$5), "done", _xlfn.DAYS(  G38, TODAY() ) )</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I38" s="21">
         <f t="shared" si="0"/>
@@ -5884,7 +5884,7 @@
       </c>
       <c r="H39" s="24">
         <f ca="1">IF(EXACT( E39, Pickers!$B$5), "done", _xlfn.DAYS(  G39, TODAY() ) )</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I39" s="21">
         <f t="shared" si="0"/>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="H40" s="24">
         <f ca="1">IF(EXACT( E40, Pickers!$B$5), "done", _xlfn.DAYS(  G40, TODAY() ) )</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I40" s="21">
         <f t="shared" si="0"/>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="H41" s="24">
         <f ca="1">IF(EXACT( E41, Pickers!$B$5), "done", _xlfn.DAYS(  G41, TODAY() ) )</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I41" s="21">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
In Class Work, organizing docs folder a little
</commit_message>
<xml_diff>
--- a/03_Docs/ReactiveSpaces-Backlog.xlsx
+++ b/03_Docs/ReactiveSpaces-Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="80">
   <si>
     <t>Plan</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Zara</t>
   </si>
   <si>
-    <t>Colour assignment</t>
-  </si>
-  <si>
     <t>Implement scoring system</t>
   </si>
   <si>
@@ -339,13 +336,13 @@
     <t>Large Dot Creation</t>
   </si>
   <si>
-    <t>Remote Interaction</t>
-  </si>
-  <si>
     <t>Large dot functionality</t>
   </si>
   <si>
     <t>Days Left</t>
+  </si>
+  <si>
+    <t>Remote Interaction &amp; Color Assignment</t>
   </si>
 </sst>
 </file>
@@ -650,7 +647,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="116">
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -675,7 +672,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
@@ -685,8 +682,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -707,7 +702,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
@@ -717,6 +712,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -742,34 +739,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -781,75 +750,10 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -875,34 +779,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -914,75 +790,10 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1008,34 +819,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1047,75 +830,10 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1141,34 +859,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1180,75 +870,10 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1274,34 +899,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1313,75 +910,10 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1402,784 +934,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2654,10 +1408,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:CB61"/>
+  <dimension ref="B2:CB60"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2673,7 +1427,7 @@
   <sheetData>
     <row r="2" spans="2:80" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -2787,7 +1541,7 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -3036,7 +1790,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:80" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3059,7 +1813,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="17">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3082,7 +1836,7 @@
         <v>14</v>
       </c>
       <c r="G11" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3098,10 +1852,14 @@
         <f>Tasks!I5-Tasks!J5</f>
         <v>7</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="16">
+        <v>14</v>
+      </c>
+      <c r="F12" s="16">
+        <v>7</v>
+      </c>
       <c r="G12" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3117,10 +1875,14 @@
         <f>Tasks!I6-Tasks!J6</f>
         <v>7</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="E13" s="16">
+        <v>14</v>
+      </c>
+      <c r="F13" s="16">
+        <v>7</v>
+      </c>
       <c r="G13" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3136,10 +1898,14 @@
         <f>Tasks!I7-Tasks!J7</f>
         <v>7</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="16">
+        <v>14</v>
+      </c>
+      <c r="F14" s="16">
+        <v>7</v>
+      </c>
       <c r="G14" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3155,10 +1921,14 @@
         <f>Tasks!I8-Tasks!J8</f>
         <v>7</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="E15" s="16">
+        <v>14</v>
+      </c>
+      <c r="F15" s="16">
+        <v>7</v>
+      </c>
       <c r="G15" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3174,10 +1944,14 @@
         <f>Tasks!I9-Tasks!J9</f>
         <v>7</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="16">
+        <v>14</v>
+      </c>
+      <c r="F16" s="16">
+        <v>7</v>
+      </c>
       <c r="G16" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3193,10 +1967,14 @@
         <f>Tasks!I10-Tasks!J10</f>
         <v>7</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="E17" s="16">
+        <v>14</v>
+      </c>
+      <c r="F17" s="16">
+        <v>7</v>
+      </c>
       <c r="G17" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3212,10 +1990,14 @@
         <f>Tasks!I11-Tasks!J11</f>
         <v>7</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="16">
+        <v>14</v>
+      </c>
+      <c r="F18" s="16">
+        <v>7</v>
+      </c>
       <c r="G18" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3231,10 +2013,14 @@
         <f>Tasks!I12-Tasks!J12</f>
         <v>7</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="E19" s="16">
+        <v>14</v>
+      </c>
+      <c r="F19" s="16">
+        <v>7</v>
+      </c>
       <c r="G19" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3250,10 +2036,14 @@
         <f>Tasks!I13-Tasks!J13</f>
         <v>7</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="E20" s="16">
+        <v>14</v>
+      </c>
+      <c r="F20" s="16">
+        <v>7</v>
+      </c>
       <c r="G20" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3269,10 +2059,14 @@
         <f>Tasks!I14-Tasks!J14</f>
         <v>7</v>
       </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="E21" s="16">
+        <v>14</v>
+      </c>
+      <c r="F21" s="16">
+        <v>7</v>
+      </c>
       <c r="G21" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3291,7 +2085,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3383,10 +2177,14 @@
         <f>Tasks!I21-Tasks!J21</f>
         <v>7</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="E27" s="16">
+        <v>7</v>
+      </c>
+      <c r="F27" s="16">
+        <v>7</v>
+      </c>
       <c r="G27" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3402,10 +2200,14 @@
         <f>Tasks!I22-Tasks!J22</f>
         <v>7</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
+      <c r="E28" s="16">
+        <v>14</v>
+      </c>
+      <c r="F28" s="16">
+        <v>7</v>
+      </c>
       <c r="G28" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3421,10 +2223,14 @@
         <f>Tasks!I23-Tasks!J23</f>
         <v>7</v>
       </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="E29" s="16">
+        <v>14</v>
+      </c>
+      <c r="F29" s="16">
+        <v>14</v>
+      </c>
       <c r="G29" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3440,16 +2246,20 @@
         <f>Tasks!I24-Tasks!J24</f>
         <v>7</v>
       </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
+      <c r="E30" s="16">
+        <v>21</v>
+      </c>
+      <c r="F30" s="16">
+        <v>7</v>
+      </c>
       <c r="G30" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="str">
         <f>Tasks!C25</f>
-        <v>Colour assignment</v>
+        <v>Remote Interaction &amp; Color Assignment</v>
       </c>
       <c r="C31" s="22">
         <f>Tasks!J25</f>
@@ -3588,15 +2398,15 @@
     <row r="35" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="str">
         <f>Tasks!C29</f>
-        <v>Remote Interaction</v>
+        <v>Create Poster, info cards</v>
       </c>
       <c r="C35" s="22">
         <f>Tasks!J29</f>
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="D35" s="22">
         <f>Tasks!I29-Tasks!J29</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
@@ -3628,20 +2438,22 @@
     <row r="36" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="15" t="str">
         <f>Tasks!C30</f>
-        <v>Create Poster, info cards</v>
+        <v>Contact lower IMD Students</v>
       </c>
       <c r="C36" s="22">
         <f>Tasks!J30</f>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D36" s="22">
         <f>Tasks!I30-Tasks!J30</f>
-        <v>7</v>
-      </c>
-      <c r="E36" s="16"/>
+        <v>12</v>
+      </c>
+      <c r="E36" s="16">
+        <v>28</v>
+      </c>
       <c r="F36" s="16"/>
       <c r="G36" s="17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H36"/>
       <c r="I36"/>
@@ -3668,20 +2480,24 @@
     <row r="37" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="str">
         <f>Tasks!C31</f>
-        <v>Contact lower IMD Students</v>
+        <v>Website - Concept</v>
       </c>
       <c r="C37" s="22">
         <f>Tasks!J31</f>
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D37" s="22">
         <f>Tasks!I31-Tasks!J31</f>
-        <v>12</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="E37" s="16">
+        <v>1</v>
+      </c>
+      <c r="F37" s="16">
+        <v>4</v>
+      </c>
       <c r="G37" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37"/>
       <c r="I37"/>
@@ -3707,21 +2523,23 @@
     </row>
     <row r="38" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="str">
-        <f>Tasks!C32</f>
-        <v>Website - Concept</v>
+        <f>Tasks!C33</f>
+        <v>Website - Final</v>
       </c>
       <c r="C38" s="22">
-        <f>Tasks!J32</f>
-        <v>1</v>
+        <f>Tasks!J33</f>
+        <v>63</v>
       </c>
       <c r="D38" s="22">
-        <f>Tasks!I32-Tasks!J32</f>
-        <v>4</v>
-      </c>
-      <c r="E38" s="16"/>
+        <f>Tasks!I33-Tasks!J33</f>
+        <v>8</v>
+      </c>
+      <c r="E38" s="16">
+        <v>21</v>
+      </c>
       <c r="F38" s="16"/>
       <c r="G38" s="17">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H38"/>
       <c r="I38"/>
@@ -3748,7 +2566,7 @@
     <row r="39" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="15" t="str">
         <f>Tasks!C34</f>
-        <v>Website - Final</v>
+        <v>Video</v>
       </c>
       <c r="C39" s="22">
         <f>Tasks!J34</f>
@@ -3788,15 +2606,15 @@
     <row r="40" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="str">
         <f>Tasks!C35</f>
-        <v>Video</v>
+        <v>Stickers</v>
       </c>
       <c r="C40" s="22">
         <f>Tasks!J35</f>
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="D40" s="22">
         <f>Tasks!I35-Tasks!J35</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
@@ -3828,15 +2646,15 @@
     <row r="41" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="str">
         <f>Tasks!C36</f>
-        <v>Stickers</v>
+        <v>Contact BIT school about demo day</v>
       </c>
       <c r="C41" s="22">
         <f>Tasks!J36</f>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D41" s="22">
         <f>Tasks!I36-Tasks!J36</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -3868,11 +2686,11 @@
     <row r="42" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="str">
         <f>Tasks!C37</f>
-        <v>Contact BIT school about demo day</v>
+        <v>Secure equipment for demo day</v>
       </c>
       <c r="C42" s="22">
         <f>Tasks!J37</f>
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D42" s="22">
         <f>Tasks!I37-Tasks!J37</f>
@@ -3908,15 +2726,15 @@
     <row r="43" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="str">
         <f>Tasks!C38</f>
-        <v>Secure equipment for demo day</v>
+        <v>Atrium - public demo</v>
       </c>
       <c r="C43" s="22">
         <f>Tasks!J38</f>
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D43" s="22">
         <f>Tasks!I38-Tasks!J38</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
@@ -3948,15 +2766,15 @@
     <row r="44" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="15" t="str">
         <f>Tasks!C39</f>
-        <v>Atrium - public demo</v>
+        <v>Find subject(s) to use API</v>
       </c>
       <c r="C44" s="22">
         <f>Tasks!J39</f>
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D44" s="22">
         <f>Tasks!I39-Tasks!J39</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
@@ -3988,11 +2806,11 @@
     <row r="45" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="15" t="str">
         <f>Tasks!C40</f>
-        <v>Find subject(s) to use API</v>
+        <v>Create user testing form evaluation</v>
       </c>
       <c r="C45" s="22">
         <f>Tasks!J40</f>
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D45" s="22">
         <f>Tasks!I40-Tasks!J40</f>
@@ -4028,15 +2846,15 @@
     <row r="46" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="15" t="str">
         <f>Tasks!C41</f>
-        <v>Create user testing form evaluation</v>
-      </c>
-      <c r="C46" s="22">
+        <v>Support subjects during development</v>
+      </c>
+      <c r="C46" s="22" t="e">
         <f>Tasks!J41</f>
-        <v>35</v>
-      </c>
-      <c r="D46" s="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D46" s="22" t="e">
         <f>Tasks!I41-Tasks!J41</f>
-        <v>12</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
@@ -4065,24 +2883,8 @@
       <c r="AA46"/>
       <c r="AB46"/>
     </row>
-    <row r="47" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="15" t="str">
-        <f>Tasks!C42</f>
-        <v>Support subjects during development</v>
-      </c>
-      <c r="C47" s="22" t="e">
-        <f>Tasks!J42</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D47" s="22" t="e">
-        <f>Tasks!I42-Tasks!J42</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="17">
-        <v>0</v>
-      </c>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B47" s="15"/>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
@@ -4107,6 +2909,11 @@
     </row>
     <row r="48" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B48" s="15"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
@@ -4129,424 +2936,447 @@
       <c r="AA48"/>
       <c r="AB48"/>
     </row>
-    <row r="49" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B49" s="15"/>
-    </row>
-    <row r="50" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+      <c r="Y49"/>
+      <c r="Z49"/>
+      <c r="AA49"/>
+      <c r="AB49"/>
+    </row>
+    <row r="50" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B50" s="15"/>
-    </row>
-    <row r="51" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50"/>
+      <c r="Y50"/>
+      <c r="Z50"/>
+      <c r="AA50"/>
+      <c r="AB50"/>
+    </row>
+    <row r="51" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B51" s="15"/>
-    </row>
-    <row r="52" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51"/>
+      <c r="Y51"/>
+      <c r="Z51"/>
+      <c r="AA51"/>
+      <c r="AB51"/>
+    </row>
+    <row r="52" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B52" s="15"/>
-    </row>
-    <row r="53" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
+      <c r="AA52"/>
+      <c r="AB52"/>
+    </row>
+    <row r="53" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+      <c r="U53"/>
+      <c r="V53"/>
+      <c r="W53"/>
+      <c r="X53"/>
+      <c r="Y53"/>
+      <c r="Z53"/>
+      <c r="AA53"/>
+      <c r="AB53"/>
+    </row>
+    <row r="54" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B54" s="15"/>
-    </row>
-    <row r="55" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+      <c r="T54"/>
+      <c r="U54"/>
+      <c r="V54"/>
+      <c r="W54"/>
+      <c r="X54"/>
+      <c r="Y54"/>
+      <c r="Z54"/>
+      <c r="AA54"/>
+      <c r="AB54"/>
+    </row>
+    <row r="55" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B55" s="15"/>
-    </row>
-    <row r="56" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55"/>
+      <c r="Y55"/>
+      <c r="Z55"/>
+      <c r="AA55"/>
+      <c r="AB55"/>
+    </row>
+    <row r="56" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B56" s="15"/>
-    </row>
-    <row r="57" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+      <c r="T56"/>
+      <c r="U56"/>
+      <c r="V56"/>
+      <c r="W56"/>
+      <c r="X56"/>
+      <c r="Y56"/>
+      <c r="Z56"/>
+      <c r="AA56"/>
+      <c r="AB56"/>
+    </row>
+    <row r="57" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B57" s="15"/>
-    </row>
-    <row r="58" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+      <c r="T57"/>
+      <c r="U57"/>
+      <c r="V57"/>
+      <c r="W57"/>
+      <c r="X57"/>
+      <c r="Y57"/>
+      <c r="Z57"/>
+      <c r="AA57"/>
+      <c r="AB57"/>
+    </row>
+    <row r="58" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B58" s="15"/>
-    </row>
-    <row r="59" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+      <c r="T58"/>
+      <c r="U58"/>
+      <c r="V58"/>
+      <c r="W58"/>
+      <c r="X58"/>
+      <c r="Y58"/>
+      <c r="Z58"/>
+      <c r="AA58"/>
+      <c r="AB58"/>
+    </row>
+    <row r="59" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B59" s="15"/>
-    </row>
-    <row r="60" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+      <c r="X59"/>
+      <c r="Y59"/>
+      <c r="Z59"/>
+      <c r="AA59"/>
+      <c r="AB59"/>
+    </row>
+    <row r="60" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B60" s="15"/>
-    </row>
-    <row r="61" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="15"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="T60"/>
+      <c r="U60"/>
+      <c r="V60"/>
+      <c r="W60"/>
+      <c r="X60"/>
+      <c r="Y60"/>
+      <c r="Z60"/>
+      <c r="AA60"/>
+      <c r="AB60"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP47">
-    <cfRule type="expression" dxfId="115" priority="120">
+  <conditionalFormatting sqref="I9:BQ46 BS9:CB46">
+    <cfRule type="expression" dxfId="27" priority="120">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="122">
+    <cfRule type="expression" dxfId="26" priority="122">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="123">
+    <cfRule type="expression" dxfId="25" priority="123">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="124">
+    <cfRule type="expression" dxfId="24" priority="124">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="125">
+    <cfRule type="expression" dxfId="23" priority="125">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="126">
+    <cfRule type="expression" dxfId="22" priority="126">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="130">
+    <cfRule type="expression" dxfId="21" priority="130">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="131">
+    <cfRule type="expression" dxfId="20" priority="131">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:BP48">
-    <cfRule type="expression" dxfId="107" priority="121">
+  <conditionalFormatting sqref="C47:BP47">
+    <cfRule type="expression" dxfId="19" priority="121">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BP8">
-    <cfRule type="expression" dxfId="106" priority="127">
+    <cfRule type="expression" dxfId="18" priority="127">
       <formula>I$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR8">
-    <cfRule type="expression" dxfId="105" priority="118">
+    <cfRule type="expression" dxfId="17" priority="118">
       <formula>BR$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT9:BT47">
-    <cfRule type="expression" dxfId="104" priority="91">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="92">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="93">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="94">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="95">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="99" priority="96">
-      <formula>BT$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="98">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="99">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BT8">
-    <cfRule type="expression" dxfId="96" priority="97">
+    <cfRule type="expression" dxfId="16" priority="97">
       <formula>BT$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BV9:BV47">
-    <cfRule type="expression" dxfId="95" priority="82">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="83">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="84">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="85">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="86">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="87">
-      <formula>BV$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="89">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="90">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BV8">
-    <cfRule type="expression" dxfId="87" priority="88">
+    <cfRule type="expression" dxfId="15" priority="88">
       <formula>BV$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BX9:BX47">
-    <cfRule type="expression" dxfId="86" priority="73">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="74">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="75">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="76">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="77">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="78">
-      <formula>BX$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="80">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="81">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BX8">
-    <cfRule type="expression" dxfId="78" priority="79">
+    <cfRule type="expression" dxfId="14" priority="79">
       <formula>BX$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ9:BZ47">
-    <cfRule type="expression" dxfId="77" priority="64">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="65">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="66">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="67">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="68">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="69">
-      <formula>BZ$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="71">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="72">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BZ8">
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="13" priority="70">
       <formula>BZ$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CB9:CB47">
-    <cfRule type="expression" dxfId="68" priority="55">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="56">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="57">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="58">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="59">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="60">
-      <formula>CB$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="62">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="63">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="CB8">
-    <cfRule type="expression" dxfId="60" priority="61">
+    <cfRule type="expression" dxfId="12" priority="61">
       <formula>CB$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ9:BQ47">
-    <cfRule type="expression" dxfId="59" priority="46">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="47">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="48">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="49">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="50">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="51">
-      <formula>BQ$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="53">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="54">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BQ8">
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="11" priority="52">
       <formula>BQ$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BS9:BS47">
-    <cfRule type="expression" dxfId="50" priority="37">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="38">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="39">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="40">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="41">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="42">
-      <formula>BS$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="44">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="45">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BS8">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="10" priority="43">
       <formula>BS$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BU9:BU47">
-    <cfRule type="expression" dxfId="41" priority="28">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="29">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="30">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="31">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="32">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="33">
-      <formula>BU$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="35">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="36">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BU8">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="9" priority="34">
       <formula>BU$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BW9:BW47">
-    <cfRule type="expression" dxfId="32" priority="19">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="20">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="21">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="22">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="23">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="24">
-      <formula>BW$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BW8">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="8" priority="25">
       <formula>BW$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BY9:BY47">
-    <cfRule type="expression" dxfId="23" priority="10">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="11">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="12">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="13">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="15">
+  <conditionalFormatting sqref="BY8">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>BY$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="17">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BY8">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>BY$8=period_selected</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CA9:CA47">
-    <cfRule type="expression" dxfId="14" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
-      <formula>CA$8=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA8">
@@ -4596,16 +3426,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5" style="19" customWidth="1"/>
-    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="3" max="3" width="31.125" customWidth="1"/>
     <col min="4" max="4" width="17.25" style="19" customWidth="1"/>
     <col min="5" max="5" width="11.25" style="19" customWidth="1"/>
     <col min="6" max="6" width="17.25" style="19" customWidth="1"/>
@@ -4614,7 +3444,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>13</v>
@@ -4626,22 +3456,22 @@
         <v>15</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4659,7 +3489,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" s="20">
         <v>41929</v>
@@ -4669,7 +3499,7 @@
         <v>done</v>
       </c>
       <c r="I2" s="21">
-        <f t="shared" ref="I2:I42" si="0">_xlfn.DAYS( G2, DATE(2014, 10, 10))</f>
+        <f t="shared" ref="I2:I41" si="0">_xlfn.DAYS( G2, DATE(2014, 10, 10))</f>
         <v>7</v>
       </c>
       <c r="J2" s="21">
@@ -4678,7 +3508,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A42" si="1">ROW() -1</f>
+        <f t="shared" ref="A3:A41" si="1">ROW() -1</f>
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -4691,7 +3521,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="20">
         <v>41929</v>
@@ -4723,7 +3553,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="20">
         <v>41929</v>
@@ -4755,7 +3585,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" s="20">
         <v>41936</v>
@@ -4769,7 +3599,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="21">
-        <f t="shared" ref="J5:J42" si="2">(I5-7) - (MOD(I5,7))</f>
+        <f t="shared" ref="J5:J41" si="2">(I5-7) - (MOD(I5,7))</f>
         <v>7</v>
       </c>
     </row>
@@ -4788,7 +3618,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="20">
         <v>41936</v>
@@ -4821,7 +3651,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G7" s="20">
         <v>41936</v>
@@ -4854,7 +3684,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" s="20">
         <v>41943</v>
@@ -4887,7 +3717,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="20">
         <v>41943</v>
@@ -4920,7 +3750,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="20">
         <v>41943</v>
@@ -4953,7 +3783,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" s="20">
         <v>41950</v>
@@ -4986,7 +3816,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="20">
         <v>41950</v>
@@ -5019,7 +3849,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G13" s="20">
         <v>41950</v>
@@ -5052,7 +3882,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G14" s="20">
         <v>41957</v>
@@ -5085,7 +3915,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="20">
         <v>41957</v>
@@ -5118,7 +3948,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="20">
@@ -5126,7 +3956,7 @@
       </c>
       <c r="H16" s="24">
         <f ca="1">IF(EXACT( E16, Pickers!$B$5), "done", _xlfn.DAYS(  G16, TODAY() ) )</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" si="0"/>
@@ -5146,13 +3976,13 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="20">
@@ -5160,7 +3990,7 @@
       </c>
       <c r="H17" s="24">
         <f ca="1">IF(EXACT( E17, Pickers!$B$5), "done", _xlfn.DAYS(  G17, TODAY() ) )</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I17" s="21">
         <f t="shared" si="0"/>
@@ -5186,7 +4016,7 @@
         <v>36</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" s="20">
         <v>41927</v>
@@ -5218,14 +4048,14 @@
         <v>38</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="20">
         <v>41936</v>
       </c>
       <c r="H19" s="24">
         <f ca="1">IF(EXACT( E19, Pickers!$B$5), "done", _xlfn.DAYS(  G19, TODAY() ) )</f>
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" si="0"/>
@@ -5251,14 +4081,14 @@
         <v>38</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="20">
         <v>41943</v>
       </c>
       <c r="H20" s="24">
         <f ca="1">IF(EXACT( E20, Pickers!$B$5), "done", _xlfn.DAYS(  G20, TODAY() ) )</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" si="0"/>
@@ -5278,13 +4108,13 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="20">
         <v>41936</v>
@@ -5311,13 +4141,13 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" s="20">
         <v>41943</v>
@@ -5344,13 +4174,13 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" s="20">
         <v>41950</v>
@@ -5377,13 +4207,13 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G24" s="20">
         <v>41950</v>
@@ -5410,20 +4240,20 @@
         <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="20">
         <v>41957</v>
       </c>
       <c r="H25" s="24">
         <f ca="1">IF(EXACT( E25, Pickers!$B$5), "done", _xlfn.DAYS(  G25, TODAY() ) )</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I25" s="21">
         <f t="shared" si="0"/>
@@ -5443,20 +4273,20 @@
         <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G26" s="20">
         <v>41964</v>
       </c>
       <c r="H26" s="24">
         <f ca="1">IF(EXACT( E26, Pickers!$B$5), "done", _xlfn.DAYS(  G26, TODAY() ) )</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I26" s="21">
         <f t="shared" si="0"/>
@@ -5476,20 +4306,20 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="20">
         <v>41964</v>
       </c>
       <c r="H27" s="24">
         <f ca="1">IF(EXACT( E27, Pickers!$B$5), "done", _xlfn.DAYS(  G27, TODAY() ) )</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I27" s="21">
         <f t="shared" si="0"/>
@@ -5509,20 +4339,20 @@
         <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>40</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" s="20">
         <v>41964</v>
       </c>
       <c r="H28" s="24">
         <f ca="1">IF(EXACT( E28, Pickers!$B$5), "done", _xlfn.DAYS(  G28, TODAY() ) )</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I28" s="21">
         <f t="shared" si="0"/>
@@ -5539,31 +4369,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G29" s="20">
-        <v>41970</v>
+        <v>41943</v>
       </c>
       <c r="H29" s="24">
         <f ca="1">IF(EXACT( E29, Pickers!$B$5), "done", _xlfn.DAYS(  G29, TODAY() ) )</f>
-        <v>21</v>
+        <v>-7</v>
       </c>
       <c r="I29" s="21">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="J29" s="21">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -5572,7 +4402,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
         <v>46</v>
@@ -5581,22 +4411,22 @@
         <v>38</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G30" s="20">
-        <v>41943</v>
+        <v>41962</v>
       </c>
       <c r="H30" s="24">
         <f ca="1">IF(EXACT( E30, Pickers!$B$5), "done", _xlfn.DAYS(  G30, TODAY() ) )</f>
-        <v>-6</v>
+        <v>12</v>
       </c>
       <c r="I30" s="21">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J30" s="21">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -5605,31 +4435,30 @@
         <v>30</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>72</v>
       </c>
       <c r="G31" s="20">
-        <v>41962</v>
-      </c>
-      <c r="H31" s="24">
+        <v>41927</v>
+      </c>
+      <c r="H31" s="24" t="str">
         <f ca="1">IF(EXACT( E31, Pickers!$B$5), "done", _xlfn.DAYS(  G31, TODAY() ) )</f>
-        <v>13</v>
+        <v>done</v>
       </c>
       <c r="I31" s="21">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J31" s="21">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -5638,19 +4467,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G32" s="20">
-        <v>41927</v>
+        <v>41936</v>
       </c>
       <c r="H32" s="24" t="str">
         <f ca="1">IF(EXACT( E32, Pickers!$B$5), "done", _xlfn.DAYS(  G32, TODAY() ) )</f>
@@ -5658,10 +4487,11 @@
       </c>
       <c r="I32" s="21">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="J32" s="21">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -5670,31 +4500,31 @@
         <v>32</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G33" s="20">
-        <v>41936</v>
-      </c>
-      <c r="H33" s="24" t="str">
+        <v>41993</v>
+      </c>
+      <c r="H33" s="24">
         <f ca="1">IF(EXACT( E33, Pickers!$B$5), "done", _xlfn.DAYS(  G33, TODAY() ) )</f>
-        <v>done</v>
+        <v>43</v>
       </c>
       <c r="I33" s="21">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="J33" s="21">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -5703,13 +4533,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>71</v>
@@ -5719,7 +4549,7 @@
       </c>
       <c r="H34" s="24">
         <f ca="1">IF(EXACT( E34, Pickers!$B$5), "done", _xlfn.DAYS(  G34, TODAY() ) )</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I34" s="21">
         <f t="shared" si="0"/>
@@ -5736,31 +4566,31 @@
         <v>34</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
         <v>52</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G35" s="20">
-        <v>41993</v>
+        <v>41943</v>
       </c>
       <c r="H35" s="24">
         <f ca="1">IF(EXACT( E35, Pickers!$B$5), "done", _xlfn.DAYS(  G35, TODAY() ) )</f>
-        <v>44</v>
+        <v>-7</v>
       </c>
       <c r="I35" s="21">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="J35" s="21">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -5769,7 +4599,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
         <v>53</v>
@@ -5778,22 +4608,22 @@
         <v>38</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G36" s="20">
-        <v>41943</v>
+        <v>41962</v>
       </c>
       <c r="H36" s="24">
         <f ca="1">IF(EXACT( E36, Pickers!$B$5), "done", _xlfn.DAYS(  G36, TODAY() ) )</f>
-        <v>-6</v>
+        <v>12</v>
       </c>
       <c r="I36" s="21">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J36" s="21">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -5802,7 +4632,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
         <v>54</v>
@@ -5811,22 +4641,22 @@
         <v>38</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G37" s="20">
-        <v>41962</v>
+        <v>41969</v>
       </c>
       <c r="H37" s="24">
         <f ca="1">IF(EXACT( E37, Pickers!$B$5), "done", _xlfn.DAYS(  G37, TODAY() ) )</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I37" s="21">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="J37" s="21">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -5835,31 +4665,31 @@
         <v>37</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>55</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G38" s="20">
-        <v>41969</v>
+        <v>41981</v>
       </c>
       <c r="H38" s="24">
         <f ca="1">IF(EXACT( E38, Pickers!$B$5), "done", _xlfn.DAYS(  G38, TODAY() ) )</f>
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="I38" s="21">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="J38" s="21">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -5868,31 +4698,31 @@
         <v>38</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G39" s="20">
-        <v>41981</v>
+        <v>41962</v>
       </c>
       <c r="H39" s="24">
         <f ca="1">IF(EXACT( E39, Pickers!$B$5), "done", _xlfn.DAYS(  G39, TODAY() ) )</f>
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="I39" s="21">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="J39" s="21">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -5901,31 +4731,31 @@
         <v>39</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
         <v>59</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G40" s="20">
-        <v>41962</v>
+        <v>41969</v>
       </c>
       <c r="H40" s="24">
         <f ca="1">IF(EXACT( E40, Pickers!$B$5), "done", _xlfn.DAYS(  G40, TODAY() ) )</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I40" s="21">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -5934,77 +4764,44 @@
         <v>40</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
         <v>60</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="20">
-        <v>41969</v>
-      </c>
-      <c r="H41" s="24">
+        <v>71</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="24" t="e">
         <f ca="1">IF(EXACT( E41, Pickers!$B$5), "done", _xlfn.DAYS(  G41, TODAY() ) )</f>
-        <v>20</v>
-      </c>
-      <c r="I41" s="21">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="J41" s="21">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H42" s="24" t="e">
-        <f ca="1">IF(EXACT( E42, Pickers!$B$5), "done", _xlfn.DAYS(  G42, TODAY() ) )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I42" s="21" t="e">
+      <c r="I41" s="21" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J42" s="21" t="e">
+      <c r="J41" s="21" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H42">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThanOrEqual">
-      <formula>0</formula>
+  <conditionalFormatting sqref="H2:H41">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"done"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
       <formula>1</formula>
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"done"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThanOrEqual">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6043,7 +4840,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E2:E42</xm:sqref>
+          <xm:sqref>E2:E41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6053,7 +4850,7 @@
           <x14:formula1>
             <xm:f>Pickers!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E42</xm:sqref>
+          <xm:sqref>E2:E41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6076,22 +4873,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated backlog, completed documentation for js client
</commit_message>
<xml_diff>
--- a/03_Docs/ReactiveSpaces-Backlog.xlsx
+++ b/03_Docs/ReactiveSpaces-Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="81">
   <si>
     <t>Plan</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Remote Interaction &amp; Color Assignment</t>
+  </si>
+  <si>
+    <t>removed, only highscores displayed</t>
   </si>
 </sst>
 </file>
@@ -1133,15 +1136,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>259080</xdr:rowOff>
+          <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1414,18 +1417,18 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.21875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="7.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.21875" style="1" customWidth="1"/>
-    <col min="9" max="28" width="2.77734375" style="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="36.25" style="2" customWidth="1"/>
+    <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
+    <col min="9" max="28" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:80" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:80" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>63</v>
       </c>
@@ -1435,7 +1438,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="2:80" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:80" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
@@ -1478,7 +1481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:80" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:80" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
@@ -1491,12 +1494,12 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:80" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:80" x14ac:dyDescent="0.3">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:80" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:80" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -1520,7 +1523,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:80" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:80" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1548,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1770,7 +1773,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="str">
         <f>Tasks!C2</f>
         <v>desktop -&gt; synced peer list</v>
@@ -1793,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:80" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:80" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="str">
         <f>Tasks!C3</f>
         <v>websocket -&gt; local kinect data</v>
@@ -1816,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="str">
         <f>Tasks!C4</f>
         <v>Javascript -&gt; local Kinect data</v>
@@ -1839,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="str">
         <f>Tasks!C5</f>
         <v xml:space="preserve">desktop -&gt; remote kinect data </v>
@@ -1862,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="str">
         <f>Tasks!C6</f>
         <v>websocket -&gt; remote kinect data</v>
@@ -1885,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="str">
         <f>Tasks!C7</f>
         <v>Javascript -&gt; remote kinect data</v>
@@ -1908,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="str">
         <f>Tasks!C8</f>
         <v>desktop -&gt; user data</v>
@@ -1931,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:80" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:80" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="str">
         <f>Tasks!C9</f>
         <v>websocket -&gt; userdata</v>
@@ -1954,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="str">
         <f>Tasks!C10</f>
         <v>Javascript -&gt; user data</v>
@@ -1977,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="str">
         <f>Tasks!C11</f>
         <v>desktop -&gt; game session info</v>
@@ -2000,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="str">
         <f>Tasks!C12</f>
         <v>websocket -&gt; game session info</v>
@@ -2023,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="str">
         <f>Tasks!C13</f>
         <v>Javascript -&gt; game session info</v>
@@ -2046,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="str">
         <f>Tasks!C14</f>
         <v>desktop -&gt; peer game sessions</v>
@@ -2069,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="str">
         <f>Tasks!C15</f>
         <v>desktop -&gt; session / peer matching</v>
@@ -2092,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="str">
         <f>Tasks!C16</f>
         <v>debug and testing feedback</v>
@@ -2111,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="str">
         <f>Tasks!C18</f>
         <v>Create Concept</v>
@@ -2134,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="str">
         <f>Tasks!C19</f>
         <v>Design visuals</v>
@@ -2157,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="str">
         <f>Tasks!C20</f>
         <v>Create Assets</v>
@@ -2180,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="15" t="str">
         <f>Tasks!C21</f>
         <v>Dot Generation</v>
@@ -2203,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="str">
         <f>Tasks!C22</f>
         <v>Colecting Dots</v>
@@ -2226,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="str">
         <f>Tasks!C23</f>
         <v>Large Dot Creation</v>
@@ -2249,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="str">
         <f>Tasks!C24</f>
         <v>Large dot functionality</v>
@@ -2272,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="str">
         <f>Tasks!C25</f>
         <v>Remote Interaction &amp; Color Assignment</v>
@@ -2293,7 +2296,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="str">
         <f>Tasks!C26</f>
         <v>Implement scoring system</v>
@@ -2335,7 +2338,7 @@
       <c r="AA32"/>
       <c r="AB32"/>
     </row>
-    <row r="33" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="str">
         <f>Tasks!C27</f>
         <v>Implement win/lose</v>
@@ -2377,7 +2380,7 @@
       <c r="AA33"/>
       <c r="AB33"/>
     </row>
-    <row r="34" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="str">
         <f>Tasks!C28</f>
         <v>Interface</v>
@@ -2419,7 +2422,7 @@
       <c r="AA34"/>
       <c r="AB34"/>
     </row>
-    <row r="35" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="str">
         <f>Tasks!C29</f>
         <v>Create Poster, info cards</v>
@@ -2463,7 +2466,7 @@
       <c r="AA35"/>
       <c r="AB35"/>
     </row>
-    <row r="36" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="15" t="str">
         <f>Tasks!C30</f>
         <v>Contact lower IMD Students</v>
@@ -2505,7 +2508,7 @@
       <c r="AA36"/>
       <c r="AB36"/>
     </row>
-    <row r="37" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="str">
         <f>Tasks!C31</f>
         <v>Website - Concept</v>
@@ -2549,7 +2552,7 @@
       <c r="AA37"/>
       <c r="AB37"/>
     </row>
-    <row r="38" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="str">
         <f>Tasks!C33</f>
         <v>Website - Final</v>
@@ -2591,7 +2594,7 @@
       <c r="AA38"/>
       <c r="AB38"/>
     </row>
-    <row r="39" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="15" t="str">
         <f>Tasks!C34</f>
         <v>Video</v>
@@ -2631,7 +2634,7 @@
       <c r="AA39"/>
       <c r="AB39"/>
     </row>
-    <row r="40" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="str">
         <f>Tasks!C35</f>
         <v>Stickers</v>
@@ -2675,7 +2678,7 @@
       <c r="AA40"/>
       <c r="AB40"/>
     </row>
-    <row r="41" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="str">
         <f>Tasks!C36</f>
         <v>Contact BIT school about demo day</v>
@@ -2715,7 +2718,7 @@
       <c r="AA41"/>
       <c r="AB41"/>
     </row>
-    <row r="42" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="str">
         <f>Tasks!C37</f>
         <v>Secure equipment for demo day</v>
@@ -2755,7 +2758,7 @@
       <c r="AA42"/>
       <c r="AB42"/>
     </row>
-    <row r="43" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="str">
         <f>Tasks!C38</f>
         <v>Atrium - public demo</v>
@@ -2795,7 +2798,7 @@
       <c r="AA43"/>
       <c r="AB43"/>
     </row>
-    <row r="44" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="15" t="str">
         <f>Tasks!C39</f>
         <v>Find subject(s) to use API</v>
@@ -2835,7 +2838,7 @@
       <c r="AA44"/>
       <c r="AB44"/>
     </row>
-    <row r="45" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="15" t="str">
         <f>Tasks!C40</f>
         <v>Create user testing form evaluation</v>
@@ -2875,7 +2878,7 @@
       <c r="AA45"/>
       <c r="AB45"/>
     </row>
-    <row r="46" spans="2:28" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="15" t="str">
         <f>Tasks!C41</f>
         <v>Support subjects during development</v>
@@ -2915,7 +2918,7 @@
       <c r="AA46"/>
       <c r="AB46"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B47" s="15"/>
       <c r="H47"/>
       <c r="I47"/>
@@ -2939,7 +2942,7 @@
       <c r="AA47"/>
       <c r="AB47"/>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B48" s="15"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -2968,7 +2971,7 @@
       <c r="AA48"/>
       <c r="AB48"/>
     </row>
-    <row r="49" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B49" s="15"/>
       <c r="C49"/>
       <c r="D49"/>
@@ -2997,7 +3000,7 @@
       <c r="AA49"/>
       <c r="AB49"/>
     </row>
-    <row r="50" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B50" s="15"/>
       <c r="C50"/>
       <c r="D50"/>
@@ -3026,7 +3029,7 @@
       <c r="AA50"/>
       <c r="AB50"/>
     </row>
-    <row r="51" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B51" s="15"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -3055,7 +3058,7 @@
       <c r="AA51"/>
       <c r="AB51"/>
     </row>
-    <row r="52" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B52" s="15"/>
       <c r="C52"/>
       <c r="D52"/>
@@ -3084,7 +3087,7 @@
       <c r="AA52"/>
       <c r="AB52"/>
     </row>
-    <row r="53" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B53" s="15"/>
       <c r="C53"/>
       <c r="D53"/>
@@ -3113,7 +3116,7 @@
       <c r="AA53"/>
       <c r="AB53"/>
     </row>
-    <row r="54" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B54" s="15"/>
       <c r="C54"/>
       <c r="D54"/>
@@ -3142,7 +3145,7 @@
       <c r="AA54"/>
       <c r="AB54"/>
     </row>
-    <row r="55" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B55" s="15"/>
       <c r="C55"/>
       <c r="D55"/>
@@ -3171,7 +3174,7 @@
       <c r="AA55"/>
       <c r="AB55"/>
     </row>
-    <row r="56" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B56" s="15"/>
       <c r="C56"/>
       <c r="D56"/>
@@ -3200,7 +3203,7 @@
       <c r="AA56"/>
       <c r="AB56"/>
     </row>
-    <row r="57" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B57" s="15"/>
       <c r="C57"/>
       <c r="D57"/>
@@ -3229,7 +3232,7 @@
       <c r="AA57"/>
       <c r="AB57"/>
     </row>
-    <row r="58" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B58" s="15"/>
       <c r="C58"/>
       <c r="D58"/>
@@ -3258,7 +3261,7 @@
       <c r="AA58"/>
       <c r="AB58"/>
     </row>
-    <row r="59" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B59" s="15"/>
       <c r="C59"/>
       <c r="D59"/>
@@ -3287,7 +3290,7 @@
       <c r="AA59"/>
       <c r="AB59"/>
     </row>
-    <row r="60" spans="2:28" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B60" s="15"/>
       <c r="C60"/>
       <c r="D60"/>
@@ -3430,15 +3433,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>14</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
+                    <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>14</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>259080</xdr:rowOff>
+                    <xdr:rowOff>257175</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3460,21 +3463,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="19" customWidth="1"/>
-    <col min="7" max="8" width="13.33203125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="31.125" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="19" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="19" customWidth="1"/>
+    <col min="6" max="6" width="29.375" style="19" customWidth="1"/>
+    <col min="7" max="8" width="13.375" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>66</v>
       </c>
@@ -3506,7 +3509,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>ROW() -1</f>
         <v>1</v>
@@ -3538,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A41" si="1">ROW() -1</f>
         <v>2</v>
@@ -3570,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -3602,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -3635,7 +3638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -3668,7 +3671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3701,7 +3704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3734,7 +3737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3767,7 +3770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3800,7 +3803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3833,7 +3836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3866,7 +3869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3899,7 +3902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3932,7 +3935,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3965,7 +3968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3988,7 +3991,7 @@
       </c>
       <c r="H16" s="24">
         <f ca="1">IF(EXACT( E16, Pickers!$B$5), "done", _xlfn.DAYS(  G16, TODAY() ) )</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" si="0"/>
@@ -3999,7 +4002,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -4022,7 +4025,7 @@
       </c>
       <c r="H17" s="24">
         <f ca="1">IF(EXACT( E17, Pickers!$B$5), "done", _xlfn.DAYS(  G17, TODAY() ) )</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I17" s="21">
         <f t="shared" si="0"/>
@@ -4033,7 +4036,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -4065,7 +4068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -4098,7 +4101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -4131,7 +4134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4164,7 +4167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -4197,7 +4200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -4230,7 +4233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -4263,7 +4266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -4275,17 +4278,17 @@
         <v>79</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G25" s="20">
         <v>41957</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="24" t="str">
         <f ca="1">IF(EXACT( E25, Pickers!$B$5), "done", _xlfn.DAYS(  G25, TODAY() ) )</f>
-        <v>-7</v>
+        <v>done</v>
       </c>
       <c r="I25" s="21">
         <f t="shared" si="0"/>
@@ -4296,7 +4299,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -4329,7 +4332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -4346,12 +4349,15 @@
       <c r="E27" s="19" t="s">
         <v>71</v>
       </c>
+      <c r="F27" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="G27" s="20">
         <v>41964</v>
       </c>
       <c r="H27" s="24">
         <f ca="1">IF(EXACT( E27, Pickers!$B$5), "done", _xlfn.DAYS(  G27, TODAY() ) )</f>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="I27" s="21">
         <f t="shared" si="0"/>
@@ -4362,7 +4368,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -4374,17 +4380,17 @@
         <v>43</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G28" s="20">
         <v>41964</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="24" t="str">
         <f ca="1">IF(EXACT( E28, Pickers!$B$5), "done", _xlfn.DAYS(  G28, TODAY() ) )</f>
-        <v>0</v>
+        <v>done</v>
       </c>
       <c r="I28" s="21">
         <f t="shared" si="0"/>
@@ -4395,7 +4401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -4428,7 +4434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -4443,14 +4449,14 @@
         <v>38</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G30" s="20">
         <v>41962</v>
       </c>
       <c r="H30" s="24">
         <f ca="1">IF(EXACT( E30, Pickers!$B$5), "done", _xlfn.DAYS(  G30, TODAY() ) )</f>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="I30" s="21">
         <f t="shared" si="0"/>
@@ -4461,7 +4467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -4493,7 +4499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -4526,7 +4532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -4548,7 +4554,7 @@
       </c>
       <c r="H33" s="24">
         <f ca="1">IF(EXACT( E33, Pickers!$B$5), "done", _xlfn.DAYS(  G33, TODAY() ) )</f>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I33" s="21">
         <f t="shared" si="0"/>
@@ -4559,7 +4565,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -4581,7 +4587,7 @@
       </c>
       <c r="H34" s="24">
         <f ca="1">IF(EXACT( E34, Pickers!$B$5), "done", _xlfn.DAYS(  G34, TODAY() ) )</f>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I34" s="21">
         <f t="shared" si="0"/>
@@ -4592,7 +4598,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -4625,7 +4631,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -4640,14 +4646,14 @@
         <v>38</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G36" s="20">
         <v>41962</v>
       </c>
-      <c r="H36" s="24">
+      <c r="H36" s="24" t="str">
         <f ca="1">IF(EXACT( E36, Pickers!$B$5), "done", _xlfn.DAYS(  G36, TODAY() ) )</f>
-        <v>-2</v>
+        <v>done</v>
       </c>
       <c r="I36" s="21">
         <f t="shared" si="0"/>
@@ -4658,7 +4664,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -4673,14 +4679,14 @@
         <v>38</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G37" s="20">
         <v>41969</v>
       </c>
       <c r="H37" s="24">
         <f ca="1">IF(EXACT( E37, Pickers!$B$5), "done", _xlfn.DAYS(  G37, TODAY() ) )</f>
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="I37" s="21">
         <f t="shared" si="0"/>
@@ -4691,7 +4697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -4713,7 +4719,7 @@
       </c>
       <c r="H38" s="24">
         <f ca="1">IF(EXACT( E38, Pickers!$B$5), "done", _xlfn.DAYS(  G38, TODAY() ) )</f>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I38" s="21">
         <f t="shared" si="0"/>
@@ -4724,7 +4730,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -4746,7 +4752,7 @@
       </c>
       <c r="H39" s="24">
         <f ca="1">IF(EXACT( E39, Pickers!$B$5), "done", _xlfn.DAYS(  G39, TODAY() ) )</f>
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="I39" s="21">
         <f t="shared" si="0"/>
@@ -4757,7 +4763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -4779,7 +4785,7 @@
       </c>
       <c r="H40" s="24">
         <f ca="1">IF(EXACT( E40, Pickers!$B$5), "done", _xlfn.DAYS(  G40, TODAY() ) )</f>
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="I40" s="21">
         <f t="shared" si="0"/>
@@ -4790,7 +4796,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -4898,27 +4904,27 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>72</v>
       </c>

</xml_diff>